<commit_message>
Write data back to excel
</commit_message>
<xml_diff>
--- a/Vtiger-CRM-E3-FW/src/test/resources/testScriptData.xlsx
+++ b/Vtiger-CRM-E3-FW/src/test/resources/testScriptData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="org" sheetId="1" r:id="rId1"/>
-    <sheet name="contacts" sheetId="2" r:id="rId2"/>
+    <sheet name="contacts" sheetId="2" r:id="rId1"/>
+    <sheet name="org" sheetId="1" r:id="rId2"/>
     <sheet name="leads" sheetId="3" r:id="rId3"/>
     <sheet name="products" sheetId="4" r:id="rId4"/>
     <sheet name="documents" sheetId="5" r:id="rId5"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ll</t>
   </si>
@@ -92,16 +92,27 @@
   </si>
   <si>
     <t>7283841234</t>
+  </si>
+  <si>
+    <t>www.thales.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,10 +156,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -163,8 +175,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,170 +459,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="395" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="J9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H2"/>
   <sheetViews>
     <sheetView zoomScale="141" workbookViewId="0">
@@ -617,6 +469,172 @@
   <sheetData>
     <row r="2" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H2" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="149" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="J9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>